<commit_message>
Update test cases and device spec & browser info
</commit_message>
<xml_diff>
--- a/assets/testsheet/rev03_testcases_20200605.xlsx
+++ b/assets/testsheet/rev03_testcases_20200605.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Test cases (Function)" sheetId="1" r:id="rId1"/>
-    <sheet name="Input data test" sheetId="6" r:id="rId2"/>
+    <sheet name="Data test" sheetId="6" r:id="rId2"/>
     <sheet name="Responsive &amp; Browser test" sheetId="5" state="hidden" r:id="rId3"/>
     <sheet name="Responsive&amp;Browser test" sheetId="7" r:id="rId4"/>
     <sheet name="Bug report" sheetId="2" r:id="rId5"/>
@@ -125,9 +125,6 @@
     <t>Intel HD Graphics 620</t>
   </si>
   <si>
-    <t>Chrome  80.0.3987.132</t>
-  </si>
-  <si>
     <t>LG V30S (LG-H930)</t>
   </si>
   <si>
@@ -230,9 +227,6 @@
   </si>
   <si>
     <t>Chrome</t>
-  </si>
-  <si>
-    <t>80.0.3987.132</t>
   </si>
   <si>
     <t>Samsung NT900X5W</t>
@@ -521,14 +515,8 @@
     <t>Firefox</t>
   </si>
   <si>
-    <t>74.0.1 (64bits)</t>
-  </si>
-  <si>
     <t>Internet 
 Explorer</t>
-  </si>
-  <si>
-    <t>11.719.18362.0</t>
   </si>
   <si>
     <t>Edge</t>
@@ -652,6 +640,18 @@
   </si>
   <si>
     <t xml:space="preserve">1. Changing the API `base` currency is available for paid plans, therefore I have to calculate the currency rate based on the default JSON file myself. (I have a free plan) </t>
+  </si>
+  <si>
+    <t>11.836.18362.0</t>
+  </si>
+  <si>
+    <t>77.0.1 (64bits)</t>
+  </si>
+  <si>
+    <t>Chrome 83.0.4103.97</t>
+  </si>
+  <si>
+    <t>83.0.4103.97</t>
   </si>
 </sst>
 </file>
@@ -2299,85 +2299,7 @@
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF008000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFFC000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF008000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFFC000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF008000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFFC000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <font>
         <b/>
@@ -2876,11 +2798,11 @@
       </c>
       <c r="I3" s="93"/>
       <c r="J3" s="92" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K3" s="93"/>
       <c r="L3" s="92" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="M3" s="93"/>
       <c r="N3" s="88"/>
@@ -2917,13 +2839,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>15</v>
@@ -2956,10 +2878,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="100" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>11</v>
@@ -2996,7 +2918,7 @@
       </c>
       <c r="C7" s="101"/>
       <c r="D7" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>11</v>
@@ -3033,10 +2955,10 @@
       </c>
       <c r="C8" s="101"/>
       <c r="D8" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>15</v>
@@ -3070,10 +2992,10 @@
       </c>
       <c r="C9" s="102"/>
       <c r="D9" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>15</v>
@@ -3106,13 +3028,13 @@
         <v>6</v>
       </c>
       <c r="C10" s="101" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>15</v>
@@ -3146,10 +3068,10 @@
       </c>
       <c r="C11" s="101"/>
       <c r="D11" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>15</v>
@@ -3183,10 +3105,10 @@
       </c>
       <c r="C12" s="101"/>
       <c r="D12" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>15</v>
@@ -3220,10 +3142,10 @@
       </c>
       <c r="C13" s="101"/>
       <c r="D13" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>90</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>15</v>
@@ -3257,10 +3179,10 @@
       </c>
       <c r="C14" s="101"/>
       <c r="D14" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>15</v>
@@ -3294,10 +3216,10 @@
       </c>
       <c r="C15" s="101"/>
       <c r="D15" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>15</v>
@@ -3331,10 +3253,10 @@
       </c>
       <c r="C16" s="102"/>
       <c r="D16" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E16" s="50" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>15</v>
@@ -3367,13 +3289,13 @@
         <v>13</v>
       </c>
       <c r="C17" s="100" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>15</v>
@@ -3407,10 +3329,10 @@
       </c>
       <c r="C18" s="101"/>
       <c r="D18" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>15</v>
@@ -3444,10 +3366,10 @@
       </c>
       <c r="C19" s="101"/>
       <c r="D19" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>15</v>
@@ -3481,10 +3403,10 @@
       </c>
       <c r="C20" s="101"/>
       <c r="D20" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>15</v>
@@ -3518,10 +3440,10 @@
       </c>
       <c r="C21" s="101"/>
       <c r="D21" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>15</v>
@@ -3555,10 +3477,10 @@
       </c>
       <c r="C22" s="101"/>
       <c r="D22" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>15</v>
@@ -3592,10 +3514,10 @@
       </c>
       <c r="C23" s="101"/>
       <c r="D23" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>15</v>
@@ -3629,10 +3551,10 @@
       </c>
       <c r="C24" s="102"/>
       <c r="D24" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>15</v>
@@ -3668,10 +3590,10 @@
         <v>13</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>15</v>
@@ -3705,10 +3627,10 @@
       </c>
       <c r="C26" s="101"/>
       <c r="D26" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>15</v>
@@ -3745,7 +3667,7 @@
         <v>19</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>15</v>
@@ -3816,37 +3738,37 @@
       </c>
       <c r="C29" s="102"/>
       <c r="D29" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L29" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="M29" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="N29" s="45" t="s">
         <v>128</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J29" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K29" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="L29" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="M29" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="N29" s="45" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="30" spans="2:14" ht="202.2" thickBot="1">
@@ -3860,7 +3782,7 @@
         <v>14</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>15</v>
@@ -3907,13 +3829,13 @@
     <mergeCell ref="L3:M3"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:M30">
-    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3927,7 +3849,7 @@
   <dimension ref="B1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3944,7 +3866,7 @@
   <sheetData>
     <row r="1" spans="2:11" ht="23.4">
       <c r="B1" s="116" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C1" s="116"/>
       <c r="D1" s="116"/>
@@ -3956,7 +3878,7 @@
     </row>
     <row r="2" spans="2:11" ht="23.4" customHeight="1">
       <c r="B2" s="117" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C2" s="117"/>
       <c r="D2" s="117"/>
@@ -3998,7 +3920,7 @@
     </row>
     <row r="7" spans="2:11" ht="21.6" thickBot="1">
       <c r="B7" s="80" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="18.600000000000001" thickBot="1">
@@ -4009,10 +3931,10 @@
         <v>2</v>
       </c>
       <c r="D8" s="112" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E8" s="87" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F8" s="109" t="s">
         <v>4</v>
@@ -4040,25 +3962,25 @@
         <v>7</v>
       </c>
       <c r="I9" s="55" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J9" s="56" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K9" s="111"/>
     </row>
     <row r="10" spans="2:11" ht="129.6">
       <c r="B10" s="64" t="s">
+        <v>163</v>
+      </c>
+      <c r="C10" s="51" t="s">
         <v>167</v>
       </c>
-      <c r="C10" s="51" t="s">
-        <v>171</v>
-      </c>
       <c r="D10" s="51" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E10" s="51" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>15</v>
@@ -4079,16 +4001,16 @@
     </row>
     <row r="11" spans="2:11" ht="87" thickBot="1">
       <c r="B11" s="65" t="s">
+        <v>165</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>173</v>
-      </c>
       <c r="E11" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>15</v>
@@ -4106,26 +4028,26 @@
         <v>15</v>
       </c>
       <c r="K11" s="46" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="21.6" thickBot="1">
       <c r="B13" s="80" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="18.600000000000001" thickBot="1">
       <c r="B14" s="103" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C14" s="94" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="112" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E14" s="87" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F14" s="109" t="s">
         <v>4</v>
@@ -4153,25 +4075,25 @@
         <v>7</v>
       </c>
       <c r="I15" s="55" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J15" s="56" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K15" s="111"/>
     </row>
     <row r="16" spans="2:11" ht="43.2">
       <c r="B16" s="106" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C16" s="51" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D16" s="51" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E16" s="51" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>15</v>
@@ -4193,13 +4115,13 @@
     <row r="17" spans="2:11" ht="43.2">
       <c r="B17" s="107"/>
       <c r="C17" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>15</v>
@@ -4221,13 +4143,13 @@
     <row r="18" spans="2:11" ht="43.2">
       <c r="B18" s="107"/>
       <c r="C18" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>15</v>
@@ -4248,16 +4170,16 @@
     </row>
     <row r="19" spans="2:11" ht="43.2">
       <c r="B19" s="107" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="E19" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>15</v>
@@ -4279,13 +4201,13 @@
     <row r="20" spans="2:11" ht="28.8">
       <c r="B20" s="107"/>
       <c r="C20" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>15</v>
@@ -4307,13 +4229,13 @@
     <row r="21" spans="2:11" ht="58.2" thickBot="1">
       <c r="B21" s="108"/>
       <c r="C21" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>15</v>
@@ -4352,46 +4274,46 @@
     <mergeCell ref="B14:B15"/>
   </mergeCells>
   <conditionalFormatting sqref="F16:H21">
-    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16:I21">
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:J21">
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10:J11">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4418,7 +4340,7 @@
   <sheetData>
     <row r="1" spans="2:8" ht="23.4">
       <c r="B1" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
@@ -4428,7 +4350,7 @@
     </row>
     <row r="2" spans="2:8" ht="23.4" customHeight="1">
       <c r="B2" s="126" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C2" s="127"/>
       <c r="D2" s="127"/>
@@ -4462,22 +4384,22 @@
     </row>
     <row r="6" spans="2:8" ht="18" customHeight="1">
       <c r="B6" s="123" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="129" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="118" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="129" t="s">
+      <c r="E6" s="118" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="118" t="s">
+      <c r="F6" s="118" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="118" t="s">
+      <c r="G6" s="118" t="s">
         <v>74</v>
-      </c>
-      <c r="F6" s="118" t="s">
-        <v>75</v>
-      </c>
-      <c r="G6" s="118" t="s">
-        <v>76</v>
       </c>
       <c r="H6" s="120" t="s">
         <v>8</v>
@@ -4503,7 +4425,7 @@
     </row>
     <row r="9" spans="2:8" ht="30" customHeight="1" thickTop="1">
       <c r="B9" s="57" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="58" t="s">
         <v>15</v>
@@ -4524,7 +4446,7 @@
     </row>
     <row r="10" spans="2:8" ht="30" customHeight="1" thickBot="1">
       <c r="B10" s="43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10" s="61" t="s">
         <v>15</v>
@@ -4577,7 +4499,7 @@
   <sheetData>
     <row r="1" spans="2:8" ht="23.4">
       <c r="B1" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
@@ -4587,7 +4509,7 @@
     </row>
     <row r="2" spans="2:8" ht="23.4" customHeight="1">
       <c r="B2" s="126" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C2" s="127"/>
       <c r="D2" s="127"/>
@@ -4621,22 +4543,22 @@
     </row>
     <row r="6" spans="2:8" ht="18" customHeight="1">
       <c r="B6" s="123" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="129" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="118" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="129" t="s">
+      <c r="E6" s="118" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="118" t="s">
+      <c r="F6" s="118" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="118" t="s">
+      <c r="G6" s="118" t="s">
         <v>74</v>
-      </c>
-      <c r="F6" s="118" t="s">
-        <v>75</v>
-      </c>
-      <c r="G6" s="118" t="s">
-        <v>76</v>
       </c>
       <c r="H6" s="120" t="s">
         <v>8</v>
@@ -4662,7 +4584,7 @@
     </row>
     <row r="9" spans="2:8" ht="30" customHeight="1" thickTop="1">
       <c r="B9" s="71" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="72" t="s">
         <v>15</v>
@@ -4683,7 +4605,7 @@
     </row>
     <row r="10" spans="2:8" ht="30" customHeight="1">
       <c r="B10" s="71" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10" s="74" t="s">
         <v>15</v>
@@ -4704,7 +4626,7 @@
     </row>
     <row r="11" spans="2:8" ht="30" customHeight="1">
       <c r="B11" s="71" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C11" s="75" t="s">
         <v>15</v>
@@ -4725,7 +4647,7 @@
     </row>
     <row r="12" spans="2:8" ht="30" customHeight="1">
       <c r="B12" s="76" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C12" s="77" t="s">
         <v>15</v>
@@ -4746,7 +4668,7 @@
     </row>
     <row r="13" spans="2:8" ht="30" customHeight="1" thickBot="1">
       <c r="B13" s="43" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C13" s="78" t="s">
         <v>15</v>
@@ -4808,16 +4730,16 @@
   <sheetData>
     <row r="1" spans="2:17" s="19" customFormat="1" ht="35.4" thickBot="1">
       <c r="B1" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>47</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>48</v>
       </c>
       <c r="F1" s="18" t="s">
         <v>23</v>
@@ -4826,34 +4748,34 @@
         <v>26</v>
       </c>
       <c r="H1" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="J1" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="K1" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="L1" s="18" t="s">
+      <c r="M1" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="N1" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="O1" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="N1" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="O1" s="18" t="s">
+      <c r="P1" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="Q1" s="18" t="s">
         <v>55</v>
-      </c>
-      <c r="Q1" s="18" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="2:17" ht="16.2" thickBot="1">
@@ -4861,7 +4783,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="86" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
@@ -4902,8 +4824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:E5"/>
+    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4926,7 +4848,7 @@
     <row r="2" spans="1:7">
       <c r="A2"/>
       <c r="B2" s="133" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C2" s="134"/>
       <c r="D2" s="134"/>
@@ -4944,7 +4866,7 @@
     <row r="4" spans="1:7">
       <c r="A4"/>
       <c r="B4" s="133" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C4" s="134"/>
       <c r="D4" s="134"/>
@@ -4960,7 +4882,7 @@
     <row r="6" spans="1:7" ht="15.6">
       <c r="A6"/>
       <c r="B6" s="139" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="140"/>
       <c r="D6" s="140"/>
@@ -4969,7 +4891,7 @@
     <row r="7" spans="1:7">
       <c r="A7"/>
       <c r="B7" s="133" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C7" s="134"/>
       <c r="D7" s="134"/>
@@ -4978,7 +4900,7 @@
     <row r="8" spans="1:7">
       <c r="A8"/>
       <c r="B8" s="133" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C8" s="134"/>
       <c r="D8" s="134"/>
@@ -4987,7 +4909,7 @@
     <row r="9" spans="1:7">
       <c r="A9"/>
       <c r="B9" s="133" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C9" s="134"/>
       <c r="D9" s="134"/>
@@ -4996,7 +4918,7 @@
     <row r="10" spans="1:7">
       <c r="A10"/>
       <c r="B10" s="133" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C10" s="134"/>
       <c r="D10" s="134"/>
@@ -5005,7 +4927,7 @@
     <row r="11" spans="1:7" ht="15" thickBot="1">
       <c r="A11"/>
       <c r="B11" s="136" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C11" s="137"/>
       <c r="D11" s="137"/>
@@ -5021,7 +4943,7 @@
     <row r="13" spans="1:7" ht="24.6" thickTop="1" thickBot="1">
       <c r="A13"/>
       <c r="B13" s="130" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" s="131"/>
       <c r="D13" s="131"/>
@@ -5039,10 +4961,10 @@
         <v>7</v>
       </c>
       <c r="F14" s="32" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G14" s="33" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" thickTop="1">
@@ -5053,16 +4975,16 @@
         <v>27</v>
       </c>
       <c r="D15" s="62" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E15" s="62" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F15" s="62" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G15" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1">
@@ -5076,13 +4998,13 @@
         <v>30</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F16" s="24" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1">
@@ -5090,19 +5012,19 @@
         <v>25</v>
       </c>
       <c r="C17" s="66" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D17" s="24" t="s">
         <v>31</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G17" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1">
@@ -5110,19 +5032,19 @@
         <v>24</v>
       </c>
       <c r="C18" s="66" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>32</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F18" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="29" t="s">
         <v>39</v>
-      </c>
-      <c r="G18" s="29" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1">
@@ -5130,19 +5052,19 @@
         <v>29</v>
       </c>
       <c r="C19" s="66" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D19" s="24" t="s">
         <v>33</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G19" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" thickBot="1">
@@ -5150,19 +5072,19 @@
         <v>26</v>
       </c>
       <c r="C20" s="67" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>34</v>
+        <v>177</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G20" s="30" t="s">
-        <v>34</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="15" thickBot="1">
@@ -5170,7 +5092,7 @@
     </row>
     <row r="22" spans="2:7" ht="24.6" thickTop="1" thickBot="1">
       <c r="B22" s="130" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C22" s="131"/>
       <c r="D22" s="131"/>
@@ -5182,10 +5104,10 @@
         <v>26</v>
       </c>
       <c r="C23" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="31" t="s">
         <v>65</v>
-      </c>
-      <c r="D23" s="31" t="s">
-        <v>66</v>
       </c>
       <c r="E23" s="37" t="s">
         <v>23</v>
@@ -5194,10 +5116,10 @@
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" thickTop="1">
       <c r="B24" s="34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D24" s="27" t="s">
         <v>27</v>
@@ -5209,13 +5131,13 @@
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1">
       <c r="B25" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="68" t="s">
+        <v>178</v>
+      </c>
+      <c r="D25" s="24" t="s">
         <v>68</v>
-      </c>
-      <c r="C25" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="D25" s="24" t="s">
-        <v>70</v>
       </c>
       <c r="E25" s="29" t="s">
         <v>30</v>
@@ -5224,13 +5146,13 @@
     </row>
     <row r="26" spans="2:7" ht="28.8">
       <c r="B26" s="34" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C26" s="68" t="s">
-        <v>142</v>
+        <v>176</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E26" s="29" t="s">
         <v>30</v>
@@ -5239,13 +5161,13 @@
     </row>
     <row r="27" spans="2:7" ht="28.8">
       <c r="B27" s="69" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C27" s="68" t="s">
-        <v>144</v>
+        <v>175</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E27" s="29" t="s">
         <v>30</v>
@@ -5254,13 +5176,13 @@
     </row>
     <row r="28" spans="2:7" ht="29.4" thickBot="1">
       <c r="B28" s="70" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C28" s="39" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E28" s="30" t="s">
         <v>30</v>

</xml_diff>